<commit_message>
Referenties nieuwe CERA-bonnen (bis)
</commit_message>
<xml_diff>
--- a/functions/vouchers/template-credit-export.xlsx
+++ b/functions/vouchers/template-credit-export.xlsx
@@ -1,30 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/frederik/Library/Mobile Documents/com~apple~CloudDocs/Sites/git-ob2c/functions/vouchers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C047EEDC-459D-3849-BD26-1C6E090A95BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{560DFB79-ABF6-1F49-8986-348D548221C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3000" yWindow="1980" windowWidth="25600" windowHeight="15540" xr2:uid="{0B9CA819-6430-064D-AB9E-0776AE783779}"/>
+    <workbookView xWindow="3000" yWindow="1980" windowWidth="25600" windowHeight="15540" activeTab="3" xr2:uid="{0B9CA819-6430-064D-AB9E-0776AE783779}"/>
   </bookViews>
   <sheets>
-    <sheet name="08935" sheetId="5" r:id="rId1"/>
-    <sheet name="08936" sheetId="6" r:id="rId2"/>
-    <sheet name="08937" sheetId="7" r:id="rId3"/>
-    <sheet name="08953" sheetId="8" r:id="rId4"/>
-    <sheet name="08954" sheetId="9" r:id="rId5"/>
+    <sheet name="08937" sheetId="7" r:id="rId1"/>
+    <sheet name="08953" sheetId="8" r:id="rId2"/>
+    <sheet name="08954" sheetId="9" r:id="rId3"/>
+    <sheet name="08955" sheetId="10" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'08935'!$A$1:$B$7</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'08936'!$A$1:$B$7</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'08937'!$A$1:$B$7</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'08953'!$A$1:$B$7</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'08954'!$A$1:$B$7</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'08937'!$A$1:$B$7</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'08953'!$A$1:$B$7</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'08954'!$A$1:$B$7</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'08955'!$A$1:$B$7</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="2">
   <si>
     <t>Winkel</t>
   </si>
@@ -106,9 +104,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Thema">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -146,7 +144,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -252,7 +250,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -394,18 +392,19 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C3DC0B8-E181-CF45-ABA2-07F466402B83}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE87E7E9-F350-F742-9611-6C94B8513391}">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="A2" sqref="A2"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -433,70 +432,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0195E8B6-828F-5A4B-B4EF-86D541E5F34F}">
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="20.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <autoFilter ref="A1:B7" xr:uid="{D28F2188-C164-1B46-B108-97876DE586EA}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B7">
-      <sortCondition ref="A1:A7"/>
-    </sortState>
-  </autoFilter>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE87E7E9-F350-F742-9611-6C94B8513391}">
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="20.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <autoFilter ref="A1:B7" xr:uid="{D28F2188-C164-1B46-B108-97876DE586EA}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B7">
-      <sortCondition ref="A1:A7"/>
-    </sortState>
-  </autoFilter>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57FEDA6D-CB5C-6242-ADA6-F89D52C97EC4}">
   <dimension ref="A1:B1"/>
   <sheetViews>
@@ -528,7 +463,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE3EE166-9859-274C-B89E-1FD4A993170B}">
   <dimension ref="A1:B1"/>
   <sheetViews>
@@ -558,4 +493,36 @@
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{143459BC-ABE2-AE41-AF86-F73634D01A3C}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="20.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:B7" xr:uid="{D28F2188-C164-1B46-B108-97876DE586EA}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B7">
+      <sortCondition ref="A1:A7"/>
+    </sortState>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Verwijder oude credit refs
</commit_message>
<xml_diff>
--- a/functions/vouchers/template-credit-export.xlsx
+++ b/functions/vouchers/template-credit-export.xlsx
@@ -1,30 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/frederik/Local Sites/ob2c/app/public/wp-content/themes/oxfam-webshop/functions/vouchers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B8EF616-E00F-5448-BFE9-0F873D62B742}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4983007D-2AE2-3F4C-B1E7-4E047F604E02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3000" yWindow="1980" windowWidth="25600" windowHeight="15540" xr2:uid="{0B9CA819-6430-064D-AB9E-0776AE783779}"/>
   </bookViews>
   <sheets>
-    <sheet name="08953" sheetId="8" r:id="rId1"/>
-    <sheet name="08954" sheetId="9" r:id="rId2"/>
-    <sheet name="08955" sheetId="10" r:id="rId3"/>
-    <sheet name="08899" sheetId="7" r:id="rId4"/>
-    <sheet name="08900" sheetId="11" r:id="rId5"/>
+    <sheet name="08955" sheetId="10" r:id="rId1"/>
+    <sheet name="08899" sheetId="7" r:id="rId2"/>
+    <sheet name="08900" sheetId="11" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'08899'!$A$1:$B$7</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'08900'!$A$1:$B$7</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'08953'!$A$1:$B$7</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'08954'!$A$1:$B$7</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'08955'!$A$1:$B$7</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'08899'!$A$1:$B$7</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'08900'!$A$1:$B$7</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'08955'!$A$1:$B$7</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="2">
   <si>
     <t>Winkel</t>
   </si>
@@ -401,7 +397,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57FEDA6D-CB5C-6242-ADA6-F89D52C97EC4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{143459BC-ABE2-AE41-AF86-F73634D01A3C}">
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -433,70 +429,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE3EE166-9859-274C-B89E-1FD4A993170B}">
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="20.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <autoFilter ref="A1:B7" xr:uid="{D28F2188-C164-1B46-B108-97876DE586EA}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B7">
-      <sortCondition ref="A1:A7"/>
-    </sortState>
-  </autoFilter>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{143459BC-ABE2-AE41-AF86-F73634D01A3C}">
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="20.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <autoFilter ref="A1:B7" xr:uid="{D28F2188-C164-1B46-B108-97876DE586EA}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B7">
-      <sortCondition ref="A1:A7"/>
-    </sortState>
-  </autoFilter>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE87E7E9-F350-F742-9611-6C94B8513391}">
   <dimension ref="A1:B1"/>
   <sheetViews>
@@ -529,7 +461,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2CD0075-D7E7-3343-8624-C1C8211B91F3}">
   <dimension ref="A1:B1"/>
   <sheetViews>

</xml_diff>